<commit_message>
Code changes gebasseerd op feedback
</commit_message>
<xml_diff>
--- a/files/Test1234/Bestand2.xlsx
+++ b/files/Test1234/Bestand2.xlsx
@@ -34,7 +34,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00500000"/>
+        <fgColor rgb="000069FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -352,9 +352,9 @@
           <t>Dit is bestand 2 column 2</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Data bestand 2Dit is bestand 1 column 2Bestand 1 column 2Bestand 1 column 3Bestand 1 column 4Bestand 1 column 5Bestand 1 column 6Bestand 1 column 7Bestand 1 column 8Bestand 1 column 9Bestand 1 column 10Bestand 1 column 11</t>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Data bestand 2</t>
         </is>
       </c>
     </row>
@@ -369,9 +369,9 @@
           <t>Bestand 2 column 2</t>
         </is>
       </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>dwaDit is bestand 1 column 2Bestand 1 column 2Bestand 1 column 3Bestand 1 column 4Bestand 1 column 5Bestand 1 column 6Bestand 1 column 7Bestand 1 column 8Bestand 1 column 9Bestand 1 column 10Bestand 1 column 11</t>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>dwa</t>
         </is>
       </c>
     </row>
@@ -386,9 +386,9 @@
           <t>Bestand 2 column 3</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>dwadwaDit is bestand 1 column 2Bestand 1 column 2Bestand 1 column 3Bestand 1 column 4Bestand 1 column 5Bestand 1 column 6Bestand 1 column 7Bestand 1 column 8Bestand 1 column 9Bestand 1 column 10Bestand 1 column 11</t>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>dwadwa</t>
         </is>
       </c>
     </row>
@@ -405,7 +405,7 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>dwadwaDit is bestand 1 column 2Bestand 1 column 2Bestand 1 column 3Bestand 1 column 4Bestand 1 column 5Bestand 1 column 6Bestand 1 column 7Bestand 1 column 8Bestand 1 column 9Bestand 1 column 10Bestand 1 column 11</t>
+          <t>dwadwaBestand 1 column 4</t>
         </is>
       </c>
     </row>
@@ -420,9 +420,9 @@
           <t>Bestand 2 column 5</t>
         </is>
       </c>
-      <c r="C5" s="1" t="inlineStr">
-        <is>
-          <t>dadaDit is bestand 1 column 2Bestand 1 column 2Bestand 1 column 3Bestand 1 column 4Bestand 1 column 5Bestand 1 column 6Bestand 1 column 7Bestand 1 column 8Bestand 1 column 9Bestand 1 column 10Bestand 1 column 11</t>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>dada</t>
         </is>
       </c>
     </row>
@@ -439,7 +439,7 @@
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>dadaDit is bestand 1 column 2Bestand 1 column 2Bestand 1 column 3Bestand 1 column 4Bestand 1 column 5Bestand 1 column 6Bestand 1 column 7Bestand 1 column 8Bestand 1 column 9Bestand 1 column 10Bestand 1 column 11</t>
+          <t>dadaBestand 1 column 6</t>
         </is>
       </c>
     </row>
@@ -456,7 +456,7 @@
       </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>adaDit is bestand 1 column 2Bestand 1 column 2Bestand 1 column 3Bestand 1 column 4Bestand 1 column 5Bestand 1 column 6Bestand 1 column 7Bestand 1 column 8Bestand 1 column 9Bestand 1 column 10Bestand 1 column 11</t>
+          <t>adaBestand 1 column 2</t>
         </is>
       </c>
     </row>
@@ -471,9 +471,9 @@
           <t>Bestand 2 column 8</t>
         </is>
       </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>adaDit is bestand 1 column 2Bestand 1 column 2Bestand 1 column 3Bestand 1 column 4Bestand 1 column 5Bestand 1 column 6Bestand 1 column 7Bestand 1 column 8Bestand 1 column 9Bestand 1 column 10Bestand 1 column 11</t>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ada</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>dadaDit is bestand 1 column 2Bestand 1 column 2Bestand 1 column 3Bestand 1 column 4Bestand 1 column 5Bestand 1 column 6Bestand 1 column 7Bestand 1 column 8Bestand 1 column 9Bestand 1 column 10Bestand 1 column 11</t>
+          <t>dadaBestand 1 column 8</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="C10" s="1" t="inlineStr">
         <is>
-          <t>dadaDit is bestand 1 column 2Bestand 1 column 2Bestand 1 column 3Bestand 1 column 4Bestand 1 column 5Bestand 1 column 6Bestand 1 column 7Bestand 1 column 8Bestand 1 column 9Bestand 1 column 10Bestand 1 column 11</t>
+          <t>dadaBestand 1 column 11</t>
         </is>
       </c>
     </row>
@@ -524,7 +524,7 @@
       </c>
       <c r="C11" s="1" t="inlineStr">
         <is>
-          <t>dadaDit is bestand 1 column 2Bestand 1 column 2Bestand 1 column 3Bestand 1 column 4Bestand 1 column 5Bestand 1 column 6Bestand 1 column 7Bestand 1 column 8Bestand 1 column 9Bestand 1 column 10Bestand 1 column 11</t>
+          <t>dadaBestand 1 column 10</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="C12" s="1" t="inlineStr">
         <is>
-          <t>adaDit is bestand 1 column 2Bestand 1 column 2Bestand 1 column 3Bestand 1 column 4Bestand 1 column 5Bestand 1 column 6Bestand 1 column 7Bestand 1 column 8Bestand 1 column 9Bestand 1 column 10Bestand 1 column 11</t>
+          <t>adaBestand 1 column 9</t>
         </is>
       </c>
     </row>

</xml_diff>